<commit_message>
Correcte datum in Excel bestand na exporteren
</commit_message>
<xml_diff>
--- a/IJC_UI/Empty.xlsx
+++ b/IJC_UI/Empty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Pion" sheetId="3" r:id="rId1"/>
@@ -341,11 +341,11 @@
     <xf numFmtId="16" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,7 +653,7 @@
   </sheetPr>
   <dimension ref="B3:J56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -671,14 +671,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="20"/>
       <c r="G3" s="4"/>
       <c r="H3" s="18"/>
@@ -1330,14 +1327,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1989,14 +1983,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2631,7 +2622,7 @@
   <dimension ref="B3:J56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,14 +2639,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2798,7 +2786,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="14"/>
       <c r="G15" s="2"/>
       <c r="H15" s="10"/>
@@ -3307,14 +3295,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3966,14 +3951,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -4607,7 +4589,7 @@
   </sheetPr>
   <dimension ref="B3:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -4625,14 +4607,11 @@
   <sheetData>
     <row r="3" spans="2:10" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21" t="str">
-        <f>"3-10-2016"</f>
-        <v>3-10-2016</v>
-      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>

</xml_diff>